<commit_message>
Solution fixed, conclusion edited
</commit_message>
<xml_diff>
--- a/Nitrogen fixation/Data_collection_for_notebook.xlsx
+++ b/Nitrogen fixation/Data_collection_for_notebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zvsta\Documents\GitHub\CSC4102020\Nitrogen fixation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yasemin\Documents\University\Honours\CSCxBRX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDB1E46-D191-4D12-9A65-7262D4166EC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041468A-8C2E-4D1E-B04A-AAD59C614ABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -10180,13 +10182,13 @@
     <tableColumn id="7" xr3:uid="{20BB9D94-22AE-4E49-93E7-FAC4CA6FE7CF}" name="Biomass (cells/mL)," dataDxfId="3">
       <calculatedColumnFormula>3*10^7*Table5[[#This Row],[Absorptivity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2522A996-272A-4C37-A3F4-66AFF041C948}" name="Biomass(g/L)" dataDxfId="2">
-      <calculatedColumnFormula>1*B2+0.023</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{2522A996-272A-4C37-A3F4-66AFF041C948}" name="Biomass(g/L)" dataDxfId="0">
+      <calculatedColumnFormula>3.2*B2+0.023</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{F76B3CBD-8E09-4145-8810-C65F670099AB}" name="Biomass" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{F76B3CBD-8E09-4145-8810-C65F670099AB}" name="Biomass" dataDxfId="2">
       <calculatedColumnFormula>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{20ED7EA2-951D-48F2-B142-8C6D53642843}" name="Glucose" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{20ED7EA2-951D-48F2-B142-8C6D53642843}" name="Glucose" dataDxfId="1">
       <calculatedColumnFormula>(D2/30)*1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10463,14 +10465,14 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -10478,12 +10480,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -10494,7 +10496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -10505,7 +10507,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -10513,12 +10515,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -10529,7 +10531,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -10540,7 +10542,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -10551,7 +10553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -10562,7 +10564,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -10573,7 +10575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -10584,7 +10586,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -10592,12 +10594,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -10608,7 +10610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -10619,7 +10621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -10630,7 +10632,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -10641,7 +10643,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -10652,7 +10654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -10660,7 +10662,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -10668,12 +10670,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -10684,7 +10686,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -10695,7 +10697,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -10706,7 +10708,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -10717,7 +10719,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -10728,7 +10730,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -10739,7 +10741,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -10763,18 +10765,18 @@
       <selection pane="bottomLeft" activeCell="E1" sqref="E1:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -10797,7 +10799,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>43857.5</v>
       </c>
@@ -10823,7 +10825,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>43858.458333333336</v>
       </c>
@@ -10849,7 +10851,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43859.458333333336</v>
       </c>
@@ -10875,7 +10877,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>43861.4375</v>
       </c>
@@ -10902,7 +10904,7 @@
         <v>343.8917073170731</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>43864.322916666664</v>
       </c>
@@ -10929,7 +10931,7 @@
         <v>102.700162601626</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>43865.3125</v>
       </c>
@@ -10956,7 +10958,7 @@
         <v>111.11382113821139</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>43866.305555555555</v>
       </c>
@@ -10983,7 +10985,7 @@
         <v>79.66276422764227</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>43867.302083333336</v>
       </c>
@@ -11010,7 +11012,7 @@
         <v>88.4770731707317</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>43868.302083333336</v>
       </c>
@@ -11037,7 +11039,7 @@
         <v>116.32227642276422</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>43857.5</v>
       </c>
@@ -11064,7 +11066,7 @@
         <v>14.75739837398374</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>43858.458333333336</v>
       </c>
@@ -11091,7 +11093,7 @@
         <v>18.363252032520325</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>43859.458333333336</v>
       </c>
@@ -11118,7 +11120,7 @@
         <v>288.0009756097561</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>43861.4375</v>
       </c>
@@ -11145,7 +11147,7 @@
         <v>309.2354471544715</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>43864.322916666664</v>
       </c>
@@ -11172,7 +11174,7 @@
         <v>76.056910569105682</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>43865.3125</v>
       </c>
@@ -11199,7 +11201,7 @@
         <v>166.20325203252028</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>43866.305555555555</v>
       </c>
@@ -11226,7 +11228,7 @@
         <v>143.3661788617886</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>43867.302083333336</v>
       </c>
@@ -11253,7 +11255,7 @@
         <v>110.71317073170732</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>43868.302083333336</v>
       </c>
@@ -11300,18 +11302,18 @@
       <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -11334,7 +11336,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>43871.541666666664</v>
       </c>
@@ -11360,7 +11362,7 @@
         <v>3.0383739837398371</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>43871.583333333336</v>
       </c>
@@ -11386,7 +11388,7 @@
         <v>3.1385365853658533</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43872.262499999997</v>
       </c>
@@ -11412,7 +11414,7 @@
         <v>2.2370731707317071</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>43872.645833333336</v>
       </c>
@@ -11438,7 +11440,7 @@
         <v>2.8380487804878043</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>43873.270833333336</v>
       </c>
@@ -11464,7 +11466,7 @@
         <v>10.250081300813006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>43873.520833333336</v>
       </c>
@@ -11490,7 +11492,7 @@
         <v>17.762276422764227</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>43874.270833333336</v>
       </c>
@@ -11516,7 +11518,7 @@
         <v>125.33691056910568</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>43874.46875</v>
       </c>
@@ -11542,7 +11544,7 @@
         <v>129.54373983739836</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>43874.677083333336</v>
       </c>
@@ -11568,7 +11570,7 @@
         <v>106.70666666666668</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>43875.270833333336</v>
       </c>
@@ -11594,7 +11596,7 @@
         <v>131.74731707317073</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>43875.447916666664</v>
       </c>
@@ -11620,7 +11622,7 @@
         <v>136.45495934959348</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>43871.541666666664</v>
       </c>
@@ -11646,7 +11648,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>43871.583333333336</v>
       </c>
@@ -11672,7 +11674,7 @@
         <v>1.2354471544715446</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>43872.262499999997</v>
       </c>
@@ -11698,7 +11700,7 @@
         <v>1.1352845528455284</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>43872.645833333336</v>
       </c>
@@ -11724,7 +11726,7 @@
         <v>1.2354471544715446</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>43873.270833333336</v>
       </c>
@@ -11750,7 +11752,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>43873.520833333336</v>
       </c>
@@ -11776,7 +11778,7 @@
         <v>1.2354471544715446</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>43874.270833333336</v>
       </c>
@@ -11802,7 +11804,7 @@
         <v>6.0432520325203241</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>43874.46875</v>
       </c>
@@ -11828,7 +11830,7 @@
         <v>2.8380487804878043</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>43874.677083333336</v>
       </c>
@@ -11854,7 +11856,7 @@
         <v>26.776910569105695</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>43875.270833333336</v>
       </c>
@@ -11880,7 +11882,7 @@
         <v>3.5391869918699186</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>43875.447916666664</v>
       </c>
@@ -11906,7 +11908,7 @@
         <v>4.8413008130081296</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>43871.541666666664</v>
       </c>
@@ -11932,7 +11934,7 @@
         <v>3.6393495934959343</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>43871.583333333336</v>
       </c>
@@ -11958,7 +11960,7 @@
         <v>7.1450406504065027</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>43872.262499942131</v>
       </c>
@@ -11984,7 +11986,7 @@
         <v>2.3372357723577233</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>43872.645833333336</v>
       </c>
@@ -12010,7 +12012,7 @@
         <v>4.1401626016260158</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>43873.270833333336</v>
       </c>
@@ -12036,7 +12038,7 @@
         <v>26.877073170731702</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>43873.520833333336</v>
       </c>
@@ -12062,7 +12064,7 @@
         <v>41.10016260162601</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>43874.270833333336</v>
       </c>
@@ -12088,7 +12090,7 @@
         <v>189.44097560975607</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>43874.46875</v>
       </c>
@@ -12114,7 +12116,7 @@
         <v>196.15186991869919</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>43874.677083333336</v>
       </c>
@@ -12140,7 +12142,7 @@
         <v>148.17398373983738</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>43875.270833333336</v>
       </c>
@@ -12166,7 +12168,7 @@
         <v>127.34016260162602</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>43875.447916608799</v>
       </c>
@@ -12192,7 +12194,7 @@
         <v>150.37756097560975</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>43871.541666666664</v>
       </c>
@@ -12218,7 +12220,7 @@
         <v>6.9447154471544712</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>43871.583333333336</v>
       </c>
@@ -12244,7 +12246,7 @@
         <v>12.453658536585365</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>43872.262499942131</v>
       </c>
@@ -12270,7 +12272,7 @@
         <v>10.450406504065041</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>43872.645833333336</v>
       </c>
@@ -12296,7 +12298,7 @@
         <v>10.650731707317075</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>43873.270833333336</v>
       </c>
@@ -12322,7 +12324,7 @@
         <v>10.75089430894309</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>43873.520833333336</v>
       </c>
@@ -12348,7 +12350,7 @@
         <v>14.75739837398374</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>43874.270833333336</v>
       </c>
@@ -12374,7 +12376,7 @@
         <v>185.83512195121949</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>43874.46875</v>
       </c>
@@ -12400,7 +12402,7 @@
         <v>173.5151219512195</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>43874.677083333336</v>
       </c>
@@ -12426,7 +12428,7 @@
         <v>144.76845528455283</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>43875.270833333336</v>
       </c>
@@ -12452,7 +12454,7 @@
         <v>127.34016260162602</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>43875.447916608799</v>
       </c>
@@ -12478,7 +12480,7 @@
         <v>153.98341463414633</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>43871.541666666664</v>
       </c>
@@ -12504,7 +12506,7 @@
         <v>34.990243902439026</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>43871.583333333336</v>
       </c>
@@ -12530,7 +12532,7 @@
         <v>36.793170731707313</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>43872.262499942131</v>
       </c>
@@ -12556,7 +12558,7 @@
         <v>44.004878048780483</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>43872.645833333336</v>
       </c>
@@ -12582,7 +12584,7 @@
         <v>38.596097560975608</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>43873.270833333336</v>
       </c>
@@ -12608,7 +12610,7 @@
         <v>56.024390243902438</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>43873.520833333336</v>
       </c>
@@ -12634,7 +12636,7 @@
         <v>47.710894308943089</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>43874.270833333336</v>
       </c>
@@ -12660,7 +12662,7 @@
         <v>202.26178861788614</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <v>43874.46875</v>
       </c>
@@ -12686,7 +12688,7 @@
         <v>183.63154471544712</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>43874.677083333336</v>
       </c>
@@ -12712,7 +12714,7 @@
         <v>119.42731707317074</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>43875.270833333336</v>
       </c>
@@ -12738,7 +12740,7 @@
         <v>171.31154471544716</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>43875.447916608799</v>
       </c>
@@ -12764,7 +12766,7 @@
         <v>107.00715447154469</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>43871.541666666664</v>
       </c>
@@ -12790,7 +12792,7 @@
         <v>18.663739837398371</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>43871.583333333336</v>
       </c>
@@ -12816,7 +12818,7 @@
         <v>20.666991869918697</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>43872.262499942131</v>
       </c>
@@ -12842,7 +12844,7 @@
         <v>12.85430894308943</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>43872.645833333336</v>
       </c>
@@ -12868,7 +12870,7 @@
         <v>11.852682926829269</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>43873.270833333336</v>
       </c>
@@ -12894,7 +12896,7 @@
         <v>11.051382113821136</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
         <v>43873.520833333336</v>
       </c>
@@ -12920,7 +12922,7 @@
         <v>7.9463414634146341</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>43874.270833333336</v>
       </c>
@@ -12946,7 +12948,7 @@
         <v>103.90211382113822</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
         <v>43874.46875</v>
       </c>
@@ -12972,7 +12974,7 @@
         <v>134.05105691056909</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
         <v>43874.677083333336</v>
       </c>
@@ -12998,7 +13000,7 @@
         <v>142.36455284552844</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
         <v>43875.270833333336</v>
       </c>
@@ -13024,7 +13026,7 @@
         <v>153.58276422764226</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
         <v>43875.447916608799</v>
       </c>
@@ -13050,94 +13052,94 @@
         <v>174.31642276422764</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88" s="2"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B96" s="2"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97" s="2"/>
     </row>
   </sheetData>
@@ -13159,18 +13161,18 @@
       <selection pane="bottomLeft" activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
@@ -13199,7 +13201,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>43875.541666666664</v>
       </c>
@@ -13231,7 +13233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>43878.277777777781</v>
       </c>
@@ -13263,7 +13265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>43878.458333333336</v>
       </c>
@@ -13295,7 +13297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>43879.277777777781</v>
       </c>
@@ -13327,7 +13329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>43879.666666666664</v>
       </c>
@@ -13359,7 +13361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>43880.277777777781</v>
       </c>
@@ -13391,7 +13393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>43880.583333333336</v>
       </c>
@@ -13423,7 +13425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>43881.277777777781</v>
       </c>
@@ -13455,7 +13457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>43875.541666666664</v>
       </c>
@@ -13485,7 +13487,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>43878.277777777781</v>
       </c>
@@ -13515,7 +13517,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>43878.458333333336</v>
       </c>
@@ -13545,7 +13547,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>43879.277777777781</v>
       </c>
@@ -13575,7 +13577,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>43879.666666666664</v>
       </c>
@@ -13605,7 +13607,7 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>43880.277777777781</v>
       </c>
@@ -13635,7 +13637,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>43880.583333333336</v>
       </c>
@@ -13665,7 +13667,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>43881.277777777781</v>
       </c>
@@ -13695,7 +13697,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>43875.541666666664</v>
       </c>
@@ -13725,7 +13727,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>43878.277777777781</v>
       </c>
@@ -13755,7 +13757,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>43878.458333333336</v>
       </c>
@@ -13785,7 +13787,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>43879.277777777781</v>
       </c>
@@ -13815,7 +13817,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>43879.666666608799</v>
       </c>
@@ -13845,7 +13847,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>43880.277777777781</v>
       </c>
@@ -13875,7 +13877,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>43880.583333333336</v>
       </c>
@@ -13905,7 +13907,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>43881.277777777781</v>
       </c>
@@ -13935,7 +13937,7 @@
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>43875.541666666664</v>
       </c>
@@ -13965,7 +13967,7 @@
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>43878.277777777781</v>
       </c>
@@ -13995,7 +13997,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>43878.458333333336</v>
       </c>
@@ -14025,7 +14027,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>43879.277777777781</v>
       </c>
@@ -14055,7 +14057,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>43879.666666608799</v>
       </c>
@@ -14085,7 +14087,7 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <v>43880.277777777781</v>
       </c>
@@ -14115,7 +14117,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>43880.583333333336</v>
       </c>
@@ -14145,7 +14147,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
         <v>43881.277777777781</v>
       </c>
@@ -14175,7 +14177,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
         <v>43875.541666666664</v>
       </c>
@@ -14205,7 +14207,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
         <v>43878.277777777781</v>
       </c>
@@ -14235,7 +14237,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
         <v>43878.458333333336</v>
       </c>
@@ -14265,7 +14267,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <v>43879.277777777781</v>
       </c>
@@ -14295,7 +14297,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10">
         <v>43879.666666608799</v>
       </c>
@@ -14325,7 +14327,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>43880.277777777781</v>
       </c>
@@ -14355,7 +14357,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
         <v>43880.583333333336</v>
       </c>
@@ -14385,7 +14387,7 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
         <v>43881.277777777781</v>
       </c>
@@ -14415,7 +14417,7 @@
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
         <v>43875.541666666664</v>
       </c>
@@ -14445,7 +14447,7 @@
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
         <v>43878.277777777781</v>
       </c>
@@ -14475,7 +14477,7 @@
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10">
         <v>43878.458333333336</v>
       </c>
@@ -14505,7 +14507,7 @@
       </c>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10">
         <v>43879.277777777781</v>
       </c>
@@ -14535,7 +14537,7 @@
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10">
         <v>43879.666666608799</v>
       </c>
@@ -14565,7 +14567,7 @@
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10">
         <v>43880.277777777781</v>
       </c>
@@ -14595,7 +14597,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10">
         <v>43880.583333333336</v>
       </c>
@@ -14625,7 +14627,7 @@
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10">
         <v>43881.277777777781</v>
       </c>
@@ -14674,20 +14676,20 @@
       <selection pane="bottomLeft" activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
@@ -14719,7 +14721,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>43885.277777777781</v>
       </c>
@@ -14755,7 +14757,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>43885.486111111109</v>
       </c>
@@ -14788,7 +14790,7 @@
         <v>2.4373983739837399</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>43886.277777777781</v>
       </c>
@@ -14824,7 +14826,7 @@
         <v>9.7492682926829257</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>43886.611111111109</v>
       </c>
@@ -14857,7 +14859,7 @@
         <v>7.4555447154471537</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>43887.277777777781</v>
       </c>
@@ -14893,7 +14895,7 @@
         <v>12.784195121951221</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>43887.506944444445</v>
       </c>
@@ -14926,7 +14928,7 @@
         <v>30.873560975609752</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>43888.277777777781</v>
       </c>
@@ -14962,7 +14964,7 @@
         <v>105.1040650406504</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>43888.465277777781</v>
       </c>
@@ -14995,7 +14997,7 @@
         <v>85.973008130081297</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>43889.277777777781</v>
       </c>
@@ -15031,7 +15033,7 @@
         <v>65.339512195121941</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>43889.465277777781</v>
       </c>
@@ -15064,7 +15066,7 @@
         <v>85.973008130081297</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>43892.277777777781</v>
       </c>
@@ -15100,7 +15102,7 @@
         <v>32.486178861788616</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>43892.465277777781</v>
       </c>
@@ -15133,7 +15135,7 @@
         <v>15.057886178861787</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>43893.277777777781</v>
       </c>
@@ -15169,7 +15171,7 @@
         <v>51.817560975609744</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>43894.277777777781</v>
       </c>
@@ -15205,7 +15207,7 @@
         <v>49.013008130081289</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>43895.277777777781</v>
       </c>
@@ -15241,7 +15243,7 @@
         <v>63.536585365853654</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>43885.277777777781</v>
       </c>
@@ -15277,7 +15279,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>43885.486111111109</v>
       </c>
@@ -15310,7 +15312,7 @@
         <v>5.041626016260162</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>43886.277777777781</v>
       </c>
@@ -15346,7 +15348,7 @@
         <v>5.3421138211382111</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>43886.611111111109</v>
       </c>
@@ -15379,7 +15381,7 @@
         <v>7.1450406504065027</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>43887.277777777781</v>
       </c>
@@ -15415,7 +15417,7 @@
         <v>11.401951219512194</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>43887.506944444445</v>
       </c>
@@ -15448,7 +15450,7 @@
         <v>26.776910569105695</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>43888.277777777781</v>
       </c>
@@ -15484,7 +15486,7 @@
         <v>85.472195121951216</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>43888.465277777781</v>
       </c>
@@ -15517,7 +15519,7 @@
         <v>79.2621138211382</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>43889.277777777781</v>
       </c>
@@ -15553,7 +15555,7 @@
         <v>59.32975609756096</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>43889.465277777781</v>
       </c>
@@ -15586,7 +15588,7 @@
         <v>79.2621138211382</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>43892.277777777781</v>
       </c>
@@ -15622,7 +15624,7 @@
         <v>14.056260162601626</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>43892.465277777781</v>
       </c>
@@ -15655,7 +15657,7 @@
         <v>6.5440650406504055</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>43893.277777777781</v>
       </c>
@@ -15691,7 +15693,7 @@
         <v>45.30699186991869</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>43894.277777777781</v>
       </c>
@@ -15727,7 +15729,7 @@
         <v>38.696260162601625</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <v>43895.277777777781</v>
       </c>
@@ -15763,7 +15765,7 @@
         <v>46.709268292682914</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>43885.277777777781</v>
       </c>
@@ -15799,7 +15801,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
         <v>43885.486111111109</v>
       </c>
@@ -15832,7 +15834,7 @@
         <v>3.5391869918699186</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
         <v>43886.277777777781</v>
       </c>
@@ -15868,7 +15870,7 @@
         <v>8.4471544715447138</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
         <v>43886.611111111109</v>
       </c>
@@ -15901,7 +15903,7 @@
         <v>8.1666991869918704</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
         <v>43887.277777777781</v>
       </c>
@@ -15937,7 +15939,7 @@
         <v>11.692422764227642</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <v>43887.506944444445</v>
       </c>
@@ -15970,7 +15972,7 @@
         <v>22.399804878048776</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10">
         <v>43888.277777777781</v>
       </c>
@@ -16006,7 +16008,7 @@
         <v>91.381788617886187</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>43888.465277777781</v>
       </c>
@@ -16039,7 +16041,7 @@
         <v>94.28650406504066</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
         <v>43889.277777777781</v>
       </c>
@@ -16075,7 +16077,7 @@
         <v>74.253983739837395</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
         <v>43889.465277777781</v>
       </c>
@@ -16108,7 +16110,7 @@
         <v>94.28650406504066</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
         <v>43892.277777777781</v>
       </c>
@@ -16144,7 +16146,7 @@
         <v>38.295609756097562</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
         <v>43892.465277777781</v>
       </c>
@@ -16177,7 +16179,7 @@
         <v>23.671869918699191</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10">
         <v>43893.277777777781</v>
       </c>
@@ -16213,7 +16215,7 @@
         <v>59.429918699186977</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10">
         <v>43894.277777777781</v>
       </c>
@@ -16249,7 +16251,7 @@
         <v>61.533333333333331</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10">
         <v>43895.277777777781</v>
       </c>
@@ -16285,7 +16287,7 @@
         <v>69.74666666666667</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10">
         <v>43885.277777777781</v>
       </c>
@@ -16322,7 +16324,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10">
         <v>43885.486111111109</v>
       </c>
@@ -16355,7 +16357,7 @@
         <v>6.0432520325203241</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10">
         <v>43886.277777777781</v>
       </c>
@@ -16391,7 +16393,7 @@
         <v>46.108292682926823</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10">
         <v>43886.611111111109</v>
       </c>
@@ -16424,7 +16426,7 @@
         <v>51.517073170731699</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="10">
         <v>43887.277777777781</v>
       </c>
@@ -16460,7 +16462,7 @@
         <v>57.877398373983731</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="10">
         <v>43887.506944444445</v>
       </c>
@@ -16493,7 +16495,7 @@
         <v>61.443186991869908</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="10">
         <v>43888.277777777781</v>
       </c>
@@ -16529,7 +16531,7 @@
         <v>83.068292682926838</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="10">
         <v>43888.465277777781</v>
       </c>
@@ -16562,7 +16564,7 @@
         <v>159.49235772357724</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="10">
         <v>43889.277777777781</v>
       </c>
@@ -16598,7 +16600,7 @@
         <v>174.51674796747966</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10">
         <v>43889.465277777781</v>
       </c>
@@ -16631,7 +16633,7 @@
         <v>159.49235772357724</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10">
         <v>43892.277777777781</v>
       </c>
@@ -16667,7 +16669,7 @@
         <v>119.12682926829268</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="10">
         <v>43892.465277777781</v>
       </c>
@@ -16700,7 +16702,7 @@
         <v>134.05105691056909</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10">
         <v>43893.277777777781</v>
       </c>
@@ -16736,7 +16738,7 @@
         <v>117.92487804878047</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="10">
         <v>43894.277777777781</v>
       </c>
@@ -16772,7 +16774,7 @@
         <v>109.71154471544715</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="10">
         <v>43895.277777777781</v>
       </c>
@@ -16808,7 +16810,7 @@
         <v>123.03317073170732</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="10">
         <v>43885.277777777781</v>
       </c>
@@ -16845,7 +16847,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="10">
         <v>43885.486111111109</v>
       </c>
@@ -16878,7 +16880,7 @@
         <v>7.2452032520325202</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="10">
         <v>43886.277777777781</v>
       </c>
@@ -16914,7 +16916,7 @@
         <v>33.888455284552848</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="10">
         <v>43886.611111111109</v>
       </c>
@@ -16947,7 +16949,7 @@
         <v>27.598243902439023</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="10">
         <v>43887.277777777781</v>
       </c>
@@ -16983,7 +16985,7 @@
         <v>41.360585365853652</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="10">
         <v>43887.506944444445</v>
       </c>
@@ -17016,7 +17018,7 @@
         <v>46.208455284552848</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="10">
         <v>43888.277777777781</v>
       </c>
@@ -17052,7 +17054,7 @@
         <v>91.882601626016267</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="10">
         <v>43888.465277777781</v>
       </c>
@@ -17085,7 +17087,7 @@
         <v>154.58439024390245</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="10">
         <v>43889.277777777781</v>
       </c>
@@ -17121,7 +17123,7 @@
         <v>144.06731707317076</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="10">
         <v>43889.465277777781</v>
       </c>
@@ -17154,7 +17156,7 @@
         <v>154.58439024390245</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="10">
         <v>43892.277777777781</v>
       </c>
@@ -17190,7 +17192,7 @@
         <v>121.33040650406504</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="10">
         <v>43892.465277777781</v>
       </c>
@@ -17223,7 +17225,7 @@
         <v>134.05105691056909</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="10">
         <v>43893.277777777781</v>
       </c>
@@ -17259,7 +17261,7 @@
         <v>126.23837398373983</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="10">
         <v>43894.277777777781</v>
       </c>
@@ -17295,7 +17297,7 @@
         <v>115.22048780487806</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="10">
         <v>43895.277777777781</v>
       </c>
@@ -17331,7 +17333,7 @@
         <v>132.54861788617887</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="10">
         <v>43885.277777777781</v>
       </c>
@@ -17368,7 +17370,7 @@
         <v>0.93495934959349591</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="10">
         <v>43885.486111111109</v>
       </c>
@@ -17401,7 +17403,7 @@
         <v>5.9430894308943083</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="10">
         <v>43886.277777777781</v>
       </c>
@@ -17437,7 +17439,7 @@
         <v>27.678373983739839</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="10">
         <v>43886.611111111109</v>
       </c>
@@ -17470,7 +17472,7 @@
         <v>26.927154471544714</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="10">
         <v>43887.277777777781</v>
       </c>
@@ -17506,7 +17508,7 @@
         <v>39.737951219512198</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="10">
         <v>43887.506944444445</v>
       </c>
@@ -17539,7 +17541,7 @@
         <v>44.956422764227632</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="10">
         <v>43888.277777777781</v>
       </c>
@@ -17575,7 +17577,7 @@
         <v>67.042276422764218</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="10">
         <v>43888.465277777781</v>
       </c>
@@ -17608,7 +17610,7 @@
         <v>136.55512195121952</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="10">
         <v>43889.277777777781</v>
       </c>
@@ -17644,7 +17646,7 @@
         <v>144.16747967479674</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="10">
         <v>43889.465277777781</v>
       </c>
@@ -17677,7 +17679,7 @@
         <v>136.55512195121952</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="10">
         <v>43892.277777777781</v>
       </c>
@@ -17713,7 +17715,7 @@
         <v>99.695284552845536</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="10">
         <v>43892.465277777781</v>
       </c>
@@ -17746,7 +17748,7 @@
         <v>118.82634146341464</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="10">
         <v>43893.277777777781</v>
       </c>
@@ -17782,7 +17784,7 @@
         <v>74.15382113821137</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="10">
         <v>43894.277777777781</v>
       </c>
@@ -17818,7 +17820,7 @@
         <v>89.078048780487805</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="10">
         <v>43895.277777777781</v>
       </c>
@@ -17872,16 +17874,16 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
@@ -17913,7 +17915,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="23">
         <v>43875.541666666664</v>
       </c>
@@ -17949,7 +17951,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="24">
         <v>43878.277777777781</v>
       </c>
@@ -17984,7 +17986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="23">
         <v>43878.458333333336</v>
       </c>
@@ -18019,7 +18021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="24">
         <v>43879.277777777781</v>
       </c>
@@ -18054,7 +18056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="23">
         <v>43879.666666666664</v>
       </c>
@@ -18089,7 +18091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="24">
         <v>43880.277777777781</v>
       </c>
@@ -18124,7 +18126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="23">
         <v>43880.583333333336</v>
       </c>
@@ -18159,7 +18161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="24">
         <v>43881.277777777781</v>
       </c>
@@ -18204,22 +18206,22 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -18251,7 +18253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -18276,7 +18278,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H16" si="0">1*B2+0.023</f>
+        <f t="shared" ref="H2:H16" si="0">3.2*B2+0.023</f>
         <v>2.3E-2</v>
       </c>
       <c r="I2">
@@ -18288,7 +18290,7 @@
         <v>333.36000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5</v>
       </c>
@@ -18306,16 +18308,16 @@
         <v>1890000</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
-        <v>8.5999999999999993E-2</v>
+        <f>3.2*B3+0.023</f>
+        <v>0.22459999999999999</v>
       </c>
       <c r="I3">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>3.4959349593495932</v>
+        <v>9.1300813008130071</v>
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>24</v>
       </c>
@@ -18340,19 +18342,19 @@
         <v>9870000</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>0.35200000000000004</v>
+        <f>3.2*B4+0.023</f>
+        <v>1.0758000000000001</v>
       </c>
       <c r="I4">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>14.308943089430896</v>
+        <v>43.731707317073173</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="1"/>
         <v>333.33333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>32</v>
       </c>
@@ -18371,15 +18373,15 @@
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>0.28920000000000001</v>
+        <v>0.87484000000000006</v>
       </c>
       <c r="I5">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>11.756097560975608</v>
+        <v>35.56260162601626</v>
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>48</v>
       </c>
@@ -18405,18 +18407,18 @@
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0.42660000000000003</v>
+        <v>1.3145200000000001</v>
       </c>
       <c r="I6">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>17.341463414634145</v>
+        <v>53.435772357723586</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
         <v>320.40000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>54</v>
       </c>
@@ -18435,15 +18437,15 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0.47500000000000003</v>
+        <v>1.4694</v>
       </c>
       <c r="I7">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>19.308943089430894</v>
+        <v>59.731707317073173</v>
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>72</v>
       </c>
@@ -18469,18 +18471,18 @@
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0.93100000000000005</v>
+        <v>2.9286000000000003</v>
       </c>
       <c r="I8">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>37.845528455284551</v>
+        <v>119.04878048780489</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
         <v>175.8</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>76.5</v>
       </c>
@@ -18499,15 +18501,15 @@
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>1.5569999999999999</v>
+        <v>4.9318</v>
       </c>
       <c r="I9">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>63.292682926829265</v>
+        <v>200.47967479674796</v>
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>96</v>
       </c>
@@ -18533,18 +18535,18 @@
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>1.452</v>
+        <v>4.5957999999999997</v>
       </c>
       <c r="I10">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>59.024390243902438</v>
+        <v>186.82113821138208</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="1"/>
         <v>24.599999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>100.5</v>
       </c>
@@ -18563,15 +18565,15 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>1.5569999999999999</v>
+        <v>4.9318</v>
       </c>
       <c r="I11">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>63.292682926829265</v>
+        <v>200.47967479674796</v>
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>144</v>
       </c>
@@ -18597,15 +18599,15 @@
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>1.2249999999999999</v>
+        <v>3.8694000000000002</v>
       </c>
       <c r="I12">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>49.796747967479661</v>
+        <v>157.29268292682926</v>
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>148.5</v>
       </c>
@@ -18628,17 +18630,17 @@
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>1.3519999999999999</v>
+        <v>4.2757999999999994</v>
       </c>
       <c r="I13">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>54.959349593495922</v>
+        <v>173.81300813008127</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>168</v>
       </c>
@@ -18664,18 +18666,18 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>1.2739999999999998</v>
+        <v>4.0261999999999993</v>
       </c>
       <c r="I14">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>51.788617886178848</v>
+        <v>163.66666666666663</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>192</v>
       </c>
@@ -18701,18 +18703,18 @@
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>1.1639999999999999</v>
+        <v>3.6742000000000004</v>
       </c>
       <c r="I15">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>47.317073170731703</v>
+        <v>149.35772357723579</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>216</v>
       </c>
@@ -18738,11 +18740,11 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>1.337</v>
+        <v>4.2278000000000002</v>
       </c>
       <c r="I16">
         <f>(1000*Table5[[#This Row],[Biomass(g/L)]])/24.6</f>
-        <v>54.349593495934954</v>
+        <v>171.86178861788616</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="1"/>

</xml_diff>